<commit_message>
Correction into the Read file function to read percentage as number. Also set.seed(10)
</commit_message>
<xml_diff>
--- a/Modelo Matenimiento/out_asignacion/c_12_Out_tareas_insturmental_incomp.xlsx
+++ b/Modelo Matenimiento/out_asignacion/c_12_Out_tareas_insturmental_incomp.xlsx
@@ -38,16 +38,16 @@
     <t>total_time</t>
   </si>
   <si>
-    <t>1011</t>
+    <t>4684</t>
   </si>
   <si>
-    <t>subest</t>
+    <t>bat</t>
   </si>
   <si>
     <t>cor-baja</t>
   </si>
   <si>
-    <t>Subestacion</t>
+    <t>29S</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -142,16 +142,16 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>1460.4000299753</v>
+        <v>1460.66797549867</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.03166666666666666</v>
       </c>
       <c r="I2" t="n">
-        <v>2.033333333333333</v>
+        <v>2.0316666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>